<commit_message>
adding multiple item- changes in productDetail() and checkcart()-> checking multi line items
</commit_message>
<xml_diff>
--- a/java/Hybrid/bin/com/styletag/testcases/InputData.xlsx
+++ b/java/Hybrid/bin/com/styletag/testcases/InputData.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="58">
   <si>
     <t xml:space="preserve">Email ID</t>
   </si>
@@ -109,12 +109,18 @@
     <t xml:space="preserve">negative scenarios2</t>
   </si>
   <si>
-    <t xml:space="preserve">LoginButton enability</t>
+    <t xml:space="preserve">LoginButton disability</t>
   </si>
   <si>
     <t xml:space="preserve">Login ID</t>
   </si>
   <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">two blankspaces in each cell (both the fields are empty)</t>
+  </si>
+  <si>
     <t xml:space="preserve">test3456</t>
   </si>
   <si>
@@ -127,55 +133,52 @@
     <t xml:space="preserve">test3456@st</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>test3456@styletag</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>.</t>
-    </r>
+    <t xml:space="preserve">test3456@styletag.</t>
   </si>
   <si>
     <t xml:space="preserve">test3456@styletag.c</t>
   </si>
   <si>
+    <t xml:space="preserve">blank emailis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test3456@styletag.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">blank passwors</t>
+  </si>
+  <si>
     <t xml:space="preserve">Test3456@.com</t>
   </si>
   <si>
     <t xml:space="preserve">@.com</t>
   </si>
   <si>
-    <t xml:space="preserve">test3456@styletag.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Invalid data</t>
+    <t xml:space="preserve">LoginButton enabled</t>
+  </si>
+  <si>
+    <t xml:space="preserve">following data are not valid for login</t>
   </si>
   <si>
     <t xml:space="preserve">styletag12</t>
   </si>
   <si>
+    <t xml:space="preserve">invalid password</t>
+  </si>
+  <si>
     <t xml:space="preserve">test34567@styletag.com</t>
   </si>
   <si>
-    <t xml:space="preserve">  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">two blankspaces indicated the end</t>
+    <t xml:space="preserve">not registered credentials</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valid data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registered data</t>
   </si>
   <si>
     <t xml:space="preserve">Search Keyword</t>
@@ -203,7 +206,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -239,6 +242,14 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -282,7 +293,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -300,6 +311,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -328,13 +343,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.5459183673469"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.9183673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.2448979591837"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="25.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -560,17 +575,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.6377551020408"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.1020408163265"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -590,7 +605,10 @@
       <c r="A3" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>31</v>
       </c>
     </row>
@@ -599,102 +617,134 @@
         <v>32</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
-        <v>33</v>
+      <c r="A5" s="0" t="s">
+        <v>34</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>36</v>
+      <c r="A8" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>31</v>
+        <v>16</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>16</v>
+      <c r="A10" s="3" t="s">
+        <v>39</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>31</v>
+        <v>40</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>39</v>
+      <c r="A11" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="s">
-        <v>40</v>
+      <c r="A12" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>41</v>
+      <c r="A13" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>31</v>
+        <v>46</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>44</v>
+      <c r="A15" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A5" r:id="rId1" display="test3456@st"/>
-    <hyperlink ref="A6" r:id="rId2" display="test3456@styletag"/>
-    <hyperlink ref="A7" r:id="rId3" display="test3456@styletag.c"/>
-    <hyperlink ref="A11" r:id="rId4" display="test3456@styletag.com"/>
-    <hyperlink ref="A13" r:id="rId5" display="test3456@styletag.com"/>
-    <hyperlink ref="A14" r:id="rId6" display="test34567@styletag.com"/>
+    <hyperlink ref="A6" r:id="rId1" display="test3456@st"/>
+    <hyperlink ref="A7" r:id="rId2" display="test3456@styletag."/>
+    <hyperlink ref="A8" r:id="rId3" display="test3456@styletag.c"/>
+    <hyperlink ref="A10" r:id="rId4" display="test3456@styletag.com"/>
+    <hyperlink ref="A14" r:id="rId5" display="test3456@styletag.com"/>
+    <hyperlink ref="A15" r:id="rId6" display="test34567@styletag.com"/>
+    <hyperlink ref="A17" r:id="rId7" display="test3456@styletag.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -719,33 +769,33 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.4132653061224"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="0" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>